<commit_message>
ny data kört lokalt 20 okt 2025
</commit_message>
<xml_diff>
--- a/data/fractal_trends_monthly.xlsx
+++ b/data/fractal_trends_monthly.xlsx
@@ -536,16 +536,16 @@
         <v>42400</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E2" t="n">
         <v>22</v>
-      </c>
-      <c r="E2" t="n">
-        <v>24</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -592,13 +592,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D3" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -645,19 +645,19 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -698,10 +698,10 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D5" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="n">
         <v>17</v>
@@ -751,14 +751,14 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D6" t="n">
+        <v>18</v>
+      </c>
+      <c r="E6" t="n">
         <v>19</v>
       </c>
-      <c r="E6" t="n">
-        <v>20</v>
-      </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
@@ -766,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -804,14 +804,14 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D7" t="n">
+        <v>16</v>
+      </c>
+      <c r="E7" t="n">
         <v>18</v>
       </c>
-      <c r="E7" t="n">
-        <v>20</v>
-      </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
@@ -857,13 +857,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D8" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -910,13 +910,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D9" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -925,7 +925,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -963,13 +963,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D10" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1016,13 +1016,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D11" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1031,13 +1031,13 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -1069,13 +1069,13 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D12" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -1122,13 +1122,13 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D13" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
@@ -1175,13 +1175,13 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D14" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -1228,13 +1228,13 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D15" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -1281,13 +1281,13 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D16" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -1305,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
@@ -1334,13 +1334,13 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D17" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -1387,13 +1387,13 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D18" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1440,13 +1440,13 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D19" t="n">
         <v>11</v>
       </c>
       <c r="E19" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1493,13 +1493,13 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D20" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1514,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
         <v>0</v>
@@ -1546,28 +1546,28 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D21" t="n">
         <v>11</v>
       </c>
       <c r="E21" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F21" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
@@ -1599,22 +1599,22 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D22" t="n">
         <v>10</v>
       </c>
       <c r="E22" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F22" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G22" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -1652,19 +1652,19 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D23" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" t="n">
+        <v>15</v>
+      </c>
+      <c r="F23" t="n">
         <v>11</v>
       </c>
-      <c r="E23" t="n">
-        <v>16</v>
-      </c>
-      <c r="F23" t="n">
-        <v>12</v>
-      </c>
       <c r="G23" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H23" t="n">
         <v>1</v>
@@ -1705,22 +1705,22 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D24" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F24" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -1755,19 +1755,19 @@
         <v>43100</v>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D25" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G25" t="n">
         <v>9</v>
@@ -1782,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" t="n">
         <v>0</v>
@@ -1808,16 +1808,16 @@
         <v>43131</v>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D26" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E26" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F26" t="n">
         <v>13</v>
@@ -1861,22 +1861,22 @@
         <v>43159</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D27" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F27" t="n">
         <v>12</v>
       </c>
       <c r="G27" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H27" t="n">
         <v>0</v>
@@ -1917,16 +1917,16 @@
         <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D28" t="n">
         <v>9</v>
       </c>
       <c r="E28" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F28" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G28" t="n">
         <v>6</v>
@@ -1970,22 +1970,22 @@
         <v>0</v>
       </c>
       <c r="C29" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D29" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F29" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G29" t="n">
         <v>7</v>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
@@ -2023,22 +2023,22 @@
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D30" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G30" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
@@ -2062,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="P30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q30" t="n">
         <v>0</v>
@@ -2076,28 +2076,28 @@
         <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D31" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31" t="n">
         <v>11</v>
       </c>
       <c r="F31" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G31" t="n">
         <v>6</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31" t="n">
         <v>0</v>
@@ -2129,7 +2129,7 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D32" t="n">
         <v>7</v>
@@ -2138,10 +2138,10 @@
         <v>12</v>
       </c>
       <c r="F32" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G32" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -2150,7 +2150,7 @@
         <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" t="n">
         <v>0</v>
@@ -2182,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D33" t="n">
         <v>8</v>
@@ -2191,7 +2191,7 @@
         <v>12</v>
       </c>
       <c r="F33" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G33" t="n">
         <v>6</v>
@@ -2235,19 +2235,19 @@
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E34" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F34" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G34" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H34" t="n">
         <v>1</v>
@@ -2288,22 +2288,22 @@
         <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D35" t="n">
         <v>7</v>
       </c>
       <c r="E35" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F35" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" t="n">
         <v>7</v>
       </c>
       <c r="H35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
@@ -2312,7 +2312,7 @@
         <v>0</v>
       </c>
       <c r="K35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L35" t="n">
         <v>0</v>
@@ -2341,22 +2341,22 @@
         <v>0</v>
       </c>
       <c r="C36" t="n">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D36" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E36" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F36" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G36" t="n">
         <v>8</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -2371,10 +2371,10 @@
         <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O36" t="n">
         <v>0</v>
@@ -2394,22 +2394,22 @@
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E37" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F37" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G37" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
@@ -2447,22 +2447,22 @@
         <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D38" t="n">
         <v>8</v>
       </c>
       <c r="E38" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F38" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G38" t="n">
         <v>8</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
@@ -2500,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D39" t="n">
         <v>7</v>
@@ -2509,10 +2509,10 @@
         <v>13</v>
       </c>
       <c r="F39" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G39" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H39" t="n">
         <v>1</v>
@@ -2553,19 +2553,19 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D40" t="n">
         <v>8</v>
       </c>
       <c r="E40" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F40" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
@@ -2574,7 +2574,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" t="n">
         <v>0</v>
@@ -2606,7 +2606,7 @@
         <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D41" t="n">
         <v>6</v>
@@ -2615,13 +2615,13 @@
         <v>12</v>
       </c>
       <c r="F41" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -2659,22 +2659,22 @@
         <v>0</v>
       </c>
       <c r="C42" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D42" t="n">
         <v>6</v>
       </c>
       <c r="E42" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F42" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G42" t="n">
         <v>6</v>
       </c>
       <c r="H42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
@@ -2712,7 +2712,7 @@
         <v>0</v>
       </c>
       <c r="C43" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D43" t="n">
         <v>6</v>
@@ -2721,7 +2721,7 @@
         <v>11</v>
       </c>
       <c r="F43" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G43" t="n">
         <v>6</v>
@@ -2765,19 +2765,19 @@
         <v>0</v>
       </c>
       <c r="C44" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D44" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F44" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G44" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H44" t="n">
         <v>1</v>
@@ -2818,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="C45" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D45" t="n">
         <v>7</v>
@@ -2827,13 +2827,13 @@
         <v>13</v>
       </c>
       <c r="F45" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G45" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
@@ -2868,19 +2868,19 @@
         <v>43738</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D46" t="n">
         <v>7</v>
       </c>
       <c r="E46" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F46" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G46" t="n">
         <v>8</v>
@@ -2924,19 +2924,19 @@
         <v>0</v>
       </c>
       <c r="C47" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D47" t="n">
+        <v>6</v>
+      </c>
+      <c r="E47" t="n">
+        <v>12</v>
+      </c>
+      <c r="F47" t="n">
+        <v>20</v>
+      </c>
+      <c r="G47" t="n">
         <v>7</v>
-      </c>
-      <c r="E47" t="n">
-        <v>13</v>
-      </c>
-      <c r="F47" t="n">
-        <v>22</v>
-      </c>
-      <c r="G47" t="n">
-        <v>8</v>
       </c>
       <c r="H47" t="n">
         <v>2</v>
@@ -2977,19 +2977,19 @@
         <v>0</v>
       </c>
       <c r="C48" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D48" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F48" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G48" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H48" t="n">
         <v>3</v>
@@ -3030,19 +3030,19 @@
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E49" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F49" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G49" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H49" t="n">
         <v>3</v>
@@ -3083,22 +3083,22 @@
         <v>0</v>
       </c>
       <c r="C50" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D50" t="n">
         <v>7</v>
       </c>
       <c r="E50" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F50" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G50" t="n">
         <v>10</v>
       </c>
       <c r="H50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
@@ -3136,19 +3136,19 @@
         <v>0</v>
       </c>
       <c r="C51" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D51" t="n">
         <v>8</v>
       </c>
       <c r="E51" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F51" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G51" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H51" t="n">
         <v>2</v>
@@ -3189,16 +3189,16 @@
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D52" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E52" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F52" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G52" t="n">
         <v>8</v>
@@ -3207,7 +3207,7 @@
         <v>2</v>
       </c>
       <c r="I52" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J52" t="n">
         <v>0</v>
@@ -3242,25 +3242,25 @@
         <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D53" t="n">
         <v>8</v>
       </c>
       <c r="E53" t="n">
+        <v>13</v>
+      </c>
+      <c r="F53" t="n">
+        <v>37</v>
+      </c>
+      <c r="G53" t="n">
         <v>14</v>
-      </c>
-      <c r="F53" t="n">
-        <v>39</v>
-      </c>
-      <c r="G53" t="n">
-        <v>15</v>
       </c>
       <c r="H53" t="n">
         <v>2</v>
       </c>
       <c r="I53" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J53" t="n">
         <v>0</v>
@@ -3295,25 +3295,25 @@
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D54" t="n">
         <v>8</v>
       </c>
       <c r="E54" t="n">
+        <v>14</v>
+      </c>
+      <c r="F54" t="n">
+        <v>39</v>
+      </c>
+      <c r="G54" t="n">
         <v>15</v>
-      </c>
-      <c r="F54" t="n">
-        <v>41</v>
-      </c>
-      <c r="G54" t="n">
-        <v>16</v>
       </c>
       <c r="H54" t="n">
         <v>2</v>
       </c>
       <c r="I54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J54" t="n">
         <v>0</v>
@@ -3345,22 +3345,22 @@
         <v>44012</v>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D55" t="n">
         <v>8</v>
       </c>
       <c r="E55" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F55" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G55" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H55" t="n">
         <v>2</v>
@@ -3401,19 +3401,19 @@
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D56" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E56" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F56" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G56" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H56" t="n">
         <v>2</v>
@@ -3454,19 +3454,19 @@
         <v>0</v>
       </c>
       <c r="C57" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D57" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E57" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F57" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G57" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H57" t="n">
         <v>1</v>
@@ -3507,25 +3507,25 @@
         <v>0</v>
       </c>
       <c r="C58" t="n">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D58" t="n">
         <v>6</v>
       </c>
       <c r="E58" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F58" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G58" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H58" t="n">
         <v>2</v>
       </c>
       <c r="I58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J58" t="n">
         <v>0</v>
@@ -3560,19 +3560,19 @@
         <v>0</v>
       </c>
       <c r="C59" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E59" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F59" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G59" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H59" t="n">
         <v>2</v>
@@ -3613,19 +3613,19 @@
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D60" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E60" t="n">
         <v>11</v>
       </c>
       <c r="F60" t="n">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G60" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H60" t="n">
         <v>2</v>
@@ -3666,22 +3666,22 @@
         <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D61" t="n">
         <v>7</v>
       </c>
       <c r="E61" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F61" t="n">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G61" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H61" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I61" t="n">
         <v>3</v>
@@ -3719,7 +3719,7 @@
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D62" t="n">
         <v>6</v>
@@ -3728,10 +3728,10 @@
         <v>10</v>
       </c>
       <c r="F62" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H62" t="n">
         <v>2</v>
@@ -3769,10 +3769,10 @@
         <v>44255</v>
       </c>
       <c r="B63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D63" t="n">
         <v>5</v>
@@ -3781,10 +3781,10 @@
         <v>9</v>
       </c>
       <c r="F63" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H63" t="n">
         <v>1</v>
@@ -3825,7 +3825,7 @@
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D64" t="n">
         <v>4</v>
@@ -3834,10 +3834,10 @@
         <v>7</v>
       </c>
       <c r="F64" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H64" t="n">
         <v>1</v>
@@ -3878,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="C65" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D65" t="n">
         <v>4</v>
@@ -3887,10 +3887,10 @@
         <v>7</v>
       </c>
       <c r="F65" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H65" t="n">
         <v>1</v>
@@ -3931,7 +3931,7 @@
         <v>0</v>
       </c>
       <c r="C66" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D66" t="n">
         <v>4</v>
@@ -3940,7 +3940,7 @@
         <v>7</v>
       </c>
       <c r="F66" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G66" t="n">
         <v>5</v>
@@ -3984,16 +3984,16 @@
         <v>0</v>
       </c>
       <c r="C67" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D67" t="n">
         <v>3</v>
       </c>
       <c r="E67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F67" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G67" t="n">
         <v>4</v>
@@ -4037,19 +4037,19 @@
         <v>0</v>
       </c>
       <c r="C68" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D68" t="n">
+        <v>4</v>
+      </c>
+      <c r="E68" t="n">
+        <v>5</v>
+      </c>
+      <c r="F68" t="n">
+        <v>26</v>
+      </c>
+      <c r="G68" t="n">
         <v>3</v>
-      </c>
-      <c r="E68" t="n">
-        <v>6</v>
-      </c>
-      <c r="F68" t="n">
-        <v>28</v>
-      </c>
-      <c r="G68" t="n">
-        <v>4</v>
       </c>
       <c r="H68" t="n">
         <v>1</v>
@@ -4090,16 +4090,16 @@
         <v>0</v>
       </c>
       <c r="C69" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D69" t="n">
         <v>3</v>
       </c>
       <c r="E69" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G69" t="n">
         <v>3</v>
@@ -4108,10 +4108,10 @@
         <v>1</v>
       </c>
       <c r="I69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J69" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K69" t="n">
         <v>0</v>
@@ -4143,7 +4143,7 @@
         <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D70" t="n">
         <v>3</v>
@@ -4152,7 +4152,7 @@
         <v>5</v>
       </c>
       <c r="F70" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G70" t="n">
         <v>3</v>
@@ -4164,7 +4164,7 @@
         <v>2</v>
       </c>
       <c r="J70" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K70" t="n">
         <v>0</v>
@@ -4196,16 +4196,16 @@
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D71" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E71" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F71" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G71" t="n">
         <v>3</v>
@@ -4217,7 +4217,7 @@
         <v>1</v>
       </c>
       <c r="J71" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K71" t="n">
         <v>0</v>
@@ -4249,16 +4249,16 @@
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D72" t="n">
         <v>4</v>
       </c>
       <c r="E72" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F72" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G72" t="n">
         <v>4</v>
@@ -4267,10 +4267,10 @@
         <v>0</v>
       </c>
       <c r="I72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J72" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K72" t="n">
         <v>0</v>
@@ -4302,16 +4302,16 @@
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D73" t="n">
         <v>4</v>
       </c>
       <c r="E73" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F73" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G73" t="n">
         <v>4</v>
@@ -4323,7 +4323,7 @@
         <v>1</v>
       </c>
       <c r="J73" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K73" t="n">
         <v>0</v>
@@ -4344,7 +4344,7 @@
         <v>0</v>
       </c>
       <c r="Q73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -4355,28 +4355,28 @@
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D74" t="n">
         <v>5</v>
       </c>
       <c r="E74" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G74" t="n">
         <v>5</v>
       </c>
       <c r="H74" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I74" t="n">
         <v>2</v>
       </c>
       <c r="J74" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K74" t="n">
         <v>0</v>
@@ -4408,16 +4408,16 @@
         <v>0</v>
       </c>
       <c r="C75" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D75" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E75" t="n">
         <v>9</v>
       </c>
       <c r="F75" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G75" t="n">
         <v>5</v>
@@ -4429,7 +4429,7 @@
         <v>2</v>
       </c>
       <c r="J75" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K75" t="n">
         <v>0</v>
@@ -4461,16 +4461,16 @@
         <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D76" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E76" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G76" t="n">
         <v>5</v>
@@ -4482,7 +4482,7 @@
         <v>2</v>
       </c>
       <c r="J76" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K76" t="n">
         <v>0</v>
@@ -4514,28 +4514,28 @@
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D77" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E77" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F77" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G77" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H77" t="n">
         <v>1</v>
       </c>
       <c r="I77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J77" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K77" t="n">
         <v>0</v>
@@ -4567,16 +4567,16 @@
         <v>0</v>
       </c>
       <c r="C78" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D78" t="n">
         <v>4</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F78" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G78" t="n">
         <v>4</v>
@@ -4588,7 +4588,7 @@
         <v>1</v>
       </c>
       <c r="J78" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K78" t="n">
         <v>0</v>
@@ -4620,19 +4620,19 @@
         <v>0</v>
       </c>
       <c r="C79" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E79" t="n">
         <v>7</v>
       </c>
       <c r="F79" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G79" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H79" t="n">
         <v>1</v>
@@ -4641,7 +4641,7 @@
         <v>1</v>
       </c>
       <c r="J79" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K79" t="n">
         <v>6</v>
@@ -4673,16 +4673,16 @@
         <v>0</v>
       </c>
       <c r="C80" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D80" t="n">
         <v>5</v>
       </c>
       <c r="E80" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F80" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G80" t="n">
         <v>4</v>
@@ -4694,10 +4694,10 @@
         <v>1</v>
       </c>
       <c r="J80" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K80" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L80" t="n">
         <v>0</v>
@@ -4726,7 +4726,7 @@
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D81" t="n">
         <v>5</v>
@@ -4735,7 +4735,7 @@
         <v>7</v>
       </c>
       <c r="F81" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G81" t="n">
         <v>7</v>
@@ -4747,10 +4747,10 @@
         <v>1</v>
       </c>
       <c r="J81" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K81" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L81" t="n">
         <v>0</v>
@@ -4779,19 +4779,19 @@
         <v>0</v>
       </c>
       <c r="C82" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D82" t="n">
         <v>5</v>
       </c>
       <c r="E82" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F82" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G82" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H82" t="n">
         <v>1</v>
@@ -4800,10 +4800,10 @@
         <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K82" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L82" t="n">
         <v>0</v>
@@ -4832,16 +4832,16 @@
         <v>0</v>
       </c>
       <c r="C83" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D83" t="n">
         <v>5</v>
       </c>
       <c r="E83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G83" t="n">
         <v>6</v>
@@ -4853,10 +4853,10 @@
         <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K83" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L83" t="n">
         <v>0</v>
@@ -4885,34 +4885,34 @@
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D84" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E84" t="n">
         <v>9</v>
       </c>
       <c r="F84" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G84" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H84" t="n">
         <v>1</v>
       </c>
       <c r="I84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J84" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K84" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L84" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M84" t="n">
         <v>0</v>
@@ -4935,22 +4935,22 @@
         <v>44926</v>
       </c>
       <c r="B85" t="n">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C85" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D85" t="n">
         <v>7</v>
       </c>
       <c r="E85" t="n">
+        <v>8</v>
+      </c>
+      <c r="F85" t="n">
+        <v>38</v>
+      </c>
+      <c r="G85" t="n">
         <v>9</v>
-      </c>
-      <c r="F85" t="n">
-        <v>41</v>
-      </c>
-      <c r="G85" t="n">
-        <v>10</v>
       </c>
       <c r="H85" t="n">
         <v>1</v>
@@ -4959,13 +4959,13 @@
         <v>2</v>
       </c>
       <c r="J85" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K85" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L85" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M85" t="n">
         <v>0</v>
@@ -4988,10 +4988,10 @@
         <v>44957</v>
       </c>
       <c r="B86" t="n">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C86" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D86" t="n">
         <v>7</v>
@@ -5000,10 +5000,10 @@
         <v>9</v>
       </c>
       <c r="F86" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G86" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H86" t="n">
         <v>1</v>
@@ -5012,13 +5012,13 @@
         <v>2</v>
       </c>
       <c r="J86" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K86" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L86" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M86" t="n">
         <v>0</v>
@@ -5041,37 +5041,37 @@
         <v>44985</v>
       </c>
       <c r="B87" t="n">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C87" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D87" t="n">
         <v>7</v>
       </c>
       <c r="E87" t="n">
+        <v>9</v>
+      </c>
+      <c r="F87" t="n">
+        <v>32</v>
+      </c>
+      <c r="G87" t="n">
+        <v>8</v>
+      </c>
+      <c r="H87" t="n">
+        <v>1</v>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="n">
+        <v>32</v>
+      </c>
+      <c r="K87" t="n">
+        <v>20</v>
+      </c>
+      <c r="L87" t="n">
         <v>10</v>
-      </c>
-      <c r="F87" t="n">
-        <v>34</v>
-      </c>
-      <c r="G87" t="n">
-        <v>9</v>
-      </c>
-      <c r="H87" t="n">
-        <v>1</v>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="n">
-        <v>34</v>
-      </c>
-      <c r="K87" t="n">
-        <v>21</v>
-      </c>
-      <c r="L87" t="n">
-        <v>11</v>
       </c>
       <c r="M87" t="n">
         <v>0</v>
@@ -5094,10 +5094,10 @@
         <v>45016</v>
       </c>
       <c r="B88" t="n">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C88" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D88" t="n">
         <v>6</v>
@@ -5106,7 +5106,7 @@
         <v>8</v>
       </c>
       <c r="F88" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G88" t="n">
         <v>8</v>
@@ -5118,13 +5118,13 @@
         <v>1</v>
       </c>
       <c r="J88" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K88" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L88" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M88" t="n">
         <v>0</v>
@@ -5147,19 +5147,19 @@
         <v>45046</v>
       </c>
       <c r="B89" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C89" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D89" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E89" t="n">
         <v>8</v>
       </c>
       <c r="F89" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G89" t="n">
         <v>8</v>
@@ -5168,13 +5168,13 @@
         <v>1</v>
       </c>
       <c r="I89" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J89" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K89" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L89" t="n">
         <v>10</v>
@@ -5200,19 +5200,19 @@
         <v>45077</v>
       </c>
       <c r="B90" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C90" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D90" t="n">
         <v>5</v>
       </c>
       <c r="E90" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G90" t="n">
         <v>6</v>
@@ -5224,13 +5224,13 @@
         <v>1</v>
       </c>
       <c r="J90" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K90" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L90" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M90" t="n">
         <v>7</v>
@@ -5253,19 +5253,19 @@
         <v>45107</v>
       </c>
       <c r="B91" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C91" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D91" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E91" t="n">
         <v>6</v>
       </c>
       <c r="F91" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G91" t="n">
         <v>7</v>
@@ -5277,16 +5277,16 @@
         <v>1</v>
       </c>
       <c r="J91" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K91" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L91" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M91" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N91" t="n">
         <v>0</v>
@@ -5306,10 +5306,10 @@
         <v>45138</v>
       </c>
       <c r="B92" t="n">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C92" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D92" t="n">
         <v>6</v>
@@ -5318,28 +5318,28 @@
         <v>8</v>
       </c>
       <c r="F92" t="n">
+        <v>23</v>
+      </c>
+      <c r="G92" t="n">
+        <v>9</v>
+      </c>
+      <c r="H92" t="n">
+        <v>1</v>
+      </c>
+      <c r="I92" t="n">
+        <v>1</v>
+      </c>
+      <c r="J92" t="n">
         <v>25</v>
       </c>
-      <c r="G92" t="n">
+      <c r="K92" t="n">
+        <v>22</v>
+      </c>
+      <c r="L92" t="n">
         <v>10</v>
       </c>
-      <c r="H92" t="n">
-        <v>1</v>
-      </c>
-      <c r="I92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J92" t="n">
-        <v>27</v>
-      </c>
-      <c r="K92" t="n">
-        <v>24</v>
-      </c>
-      <c r="L92" t="n">
-        <v>11</v>
-      </c>
       <c r="M92" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N92" t="n">
         <v>0</v>
@@ -5359,19 +5359,19 @@
         <v>45169</v>
       </c>
       <c r="B93" t="n">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C93" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D93" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E93" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F93" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G93" t="n">
         <v>7</v>
@@ -5380,19 +5380,19 @@
         <v>1</v>
       </c>
       <c r="I93" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J93" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K93" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L93" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M93" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N93" t="n">
         <v>0</v>
@@ -5412,23 +5412,23 @@
         <v>45199</v>
       </c>
       <c r="B94" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C94" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D94" t="n">
+        <v>5</v>
+      </c>
+      <c r="E94" t="n">
+        <v>8</v>
+      </c>
+      <c r="F94" t="n">
+        <v>21</v>
+      </c>
+      <c r="G94" t="n">
         <v>6</v>
       </c>
-      <c r="E94" t="n">
-        <v>9</v>
-      </c>
-      <c r="F94" t="n">
-        <v>23</v>
-      </c>
-      <c r="G94" t="n">
-        <v>7</v>
-      </c>
       <c r="H94" t="n">
         <v>1</v>
       </c>
@@ -5436,16 +5436,16 @@
         <v>1</v>
       </c>
       <c r="J94" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K94" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L94" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M94" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N94" t="n">
         <v>0</v>
@@ -5465,19 +5465,19 @@
         <v>45230</v>
       </c>
       <c r="B95" t="n">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C95" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D95" t="n">
         <v>6</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G95" t="n">
         <v>6</v>
@@ -5489,16 +5489,16 @@
         <v>1</v>
       </c>
       <c r="J95" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K95" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L95" t="n">
         <v>10</v>
       </c>
       <c r="M95" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N95" t="n">
         <v>0</v>
@@ -5518,23 +5518,23 @@
         <v>45260</v>
       </c>
       <c r="B96" t="n">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C96" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D96" t="n">
+        <v>6</v>
+      </c>
+      <c r="E96" t="n">
+        <v>8</v>
+      </c>
+      <c r="F96" t="n">
+        <v>25</v>
+      </c>
+      <c r="G96" t="n">
         <v>7</v>
       </c>
-      <c r="E96" t="n">
-        <v>9</v>
-      </c>
-      <c r="F96" t="n">
-        <v>27</v>
-      </c>
-      <c r="G96" t="n">
-        <v>8</v>
-      </c>
       <c r="H96" t="n">
         <v>1</v>
       </c>
@@ -5542,16 +5542,16 @@
         <v>1</v>
       </c>
       <c r="J96" t="n">
+        <v>22</v>
+      </c>
+      <c r="K96" t="n">
         <v>24</v>
       </c>
-      <c r="K96" t="n">
-        <v>26</v>
-      </c>
       <c r="L96" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M96" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N96" t="n">
         <v>0</v>
@@ -5571,22 +5571,22 @@
         <v>45291</v>
       </c>
       <c r="B97" t="n">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C97" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D97" t="n">
         <v>6</v>
       </c>
       <c r="E97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F97" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G97" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H97" t="n">
         <v>1</v>
@@ -5595,16 +5595,16 @@
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K97" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L97" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M97" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N97" t="n">
         <v>0</v>
@@ -5624,19 +5624,19 @@
         <v>45322</v>
       </c>
       <c r="B98" t="n">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C98" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D98" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F98" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G98" t="n">
         <v>7</v>
@@ -5648,16 +5648,16 @@
         <v>1</v>
       </c>
       <c r="J98" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K98" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L98" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M98" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N98" t="n">
         <v>0</v>
@@ -5677,19 +5677,19 @@
         <v>45351</v>
       </c>
       <c r="B99" t="n">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C99" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D99" t="n">
         <v>7</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F99" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G99" t="n">
         <v>7</v>
@@ -5701,16 +5701,16 @@
         <v>2</v>
       </c>
       <c r="J99" t="n">
+        <v>19</v>
+      </c>
+      <c r="K99" t="n">
         <v>21</v>
       </c>
-      <c r="K99" t="n">
-        <v>23</v>
-      </c>
       <c r="L99" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M99" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="N99" t="n">
         <v>0</v>
@@ -5730,22 +5730,22 @@
         <v>45382</v>
       </c>
       <c r="B100" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C100" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D100" t="n">
         <v>6</v>
       </c>
       <c r="E100" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F100" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G100" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H100" t="n">
         <v>1</v>
@@ -5754,16 +5754,16 @@
         <v>1</v>
       </c>
       <c r="J100" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K100" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L100" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M100" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N100" t="n">
         <v>0</v>
@@ -5783,22 +5783,22 @@
         <v>45412</v>
       </c>
       <c r="B101" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C101" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D101" t="n">
         <v>6</v>
       </c>
       <c r="E101" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F101" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G101" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H101" t="n">
         <v>1</v>
@@ -5807,16 +5807,16 @@
         <v>1</v>
       </c>
       <c r="J101" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K101" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L101" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M101" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N101" t="n">
         <v>0</v>
@@ -5836,10 +5836,10 @@
         <v>45443</v>
       </c>
       <c r="B102" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C102" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D102" t="n">
         <v>5</v>
@@ -5848,7 +5848,7 @@
         <v>7</v>
       </c>
       <c r="F102" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G102" t="n">
         <v>5</v>
@@ -5860,16 +5860,16 @@
         <v>1</v>
       </c>
       <c r="J102" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K102" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L102" t="n">
         <v>10</v>
       </c>
       <c r="M102" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N102" t="n">
         <v>0</v>
@@ -5889,43 +5889,43 @@
         <v>45473</v>
       </c>
       <c r="B103" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C103" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D103" t="n">
         <v>6</v>
       </c>
       <c r="E103" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F103" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G103" t="n">
         <v>5</v>
       </c>
       <c r="H103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I103" t="n">
         <v>10</v>
       </c>
       <c r="J103" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K103" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L103" t="n">
         <v>12</v>
       </c>
       <c r="M103" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N103" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O103" t="n">
         <v>0</v>
@@ -5934,7 +5934,7 @@
         <v>2</v>
       </c>
       <c r="Q103" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
@@ -5942,40 +5942,40 @@
         <v>45504</v>
       </c>
       <c r="B104" t="n">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C104" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D104" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E104" t="n">
         <v>7</v>
       </c>
       <c r="F104" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G104" t="n">
         <v>5</v>
       </c>
       <c r="H104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I104" t="n">
         <v>4</v>
       </c>
       <c r="J104" t="n">
+        <v>16</v>
+      </c>
+      <c r="K104" t="n">
         <v>17</v>
       </c>
-      <c r="K104" t="n">
-        <v>18</v>
-      </c>
       <c r="L104" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M104" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N104" t="n">
         <v>9</v>
@@ -5995,40 +5995,40 @@
         <v>45535</v>
       </c>
       <c r="B105" t="n">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C105" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D105" t="n">
         <v>4</v>
       </c>
       <c r="E105" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F105" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G105" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H105" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I105" t="n">
         <v>4</v>
       </c>
       <c r="J105" t="n">
+        <v>17</v>
+      </c>
+      <c r="K105" t="n">
         <v>18</v>
       </c>
-      <c r="K105" t="n">
-        <v>19</v>
-      </c>
       <c r="L105" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M105" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N105" t="n">
         <v>6</v>
@@ -6048,19 +6048,19 @@
         <v>45565</v>
       </c>
       <c r="B106" t="n">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C106" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D106" t="n">
         <v>7</v>
       </c>
       <c r="E106" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F106" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G106" t="n">
         <v>6</v>
@@ -6069,19 +6069,19 @@
         <v>1</v>
       </c>
       <c r="I106" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J106" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K106" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L106" t="n">
         <v>11</v>
       </c>
       <c r="M106" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N106" t="n">
         <v>5</v>
@@ -6090,10 +6090,10 @@
         <v>0</v>
       </c>
       <c r="P106" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -6101,19 +6101,19 @@
         <v>45596</v>
       </c>
       <c r="B107" t="n">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C107" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D107" t="n">
         <v>7</v>
       </c>
       <c r="E107" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F107" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G107" t="n">
         <v>6</v>
@@ -6125,16 +6125,16 @@
         <v>8</v>
       </c>
       <c r="J107" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K107" t="n">
         <v>19</v>
       </c>
       <c r="L107" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M107" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N107" t="n">
         <v>5</v>
@@ -6143,7 +6143,7 @@
         <v>0</v>
       </c>
       <c r="P107" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q107" t="n">
         <v>1</v>
@@ -6154,19 +6154,19 @@
         <v>45626</v>
       </c>
       <c r="B108" t="n">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C108" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D108" t="n">
+        <v>8</v>
+      </c>
+      <c r="E108" t="n">
         <v>9</v>
       </c>
-      <c r="E108" t="n">
-        <v>10</v>
-      </c>
       <c r="F108" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G108" t="n">
         <v>8</v>
@@ -6178,16 +6178,16 @@
         <v>8</v>
       </c>
       <c r="J108" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K108" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L108" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M108" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="N108" t="n">
         <v>5</v>
@@ -6196,7 +6196,7 @@
         <v>0</v>
       </c>
       <c r="P108" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q108" t="n">
         <v>1</v>
@@ -6207,40 +6207,40 @@
         <v>45657</v>
       </c>
       <c r="B109" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C109" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D109" t="n">
+        <v>8</v>
+      </c>
+      <c r="E109" t="n">
+        <v>11</v>
+      </c>
+      <c r="F109" t="n">
+        <v>28</v>
+      </c>
+      <c r="G109" t="n">
         <v>9</v>
       </c>
-      <c r="E109" t="n">
-        <v>12</v>
-      </c>
-      <c r="F109" t="n">
-        <v>31</v>
-      </c>
-      <c r="G109" t="n">
-        <v>10</v>
-      </c>
       <c r="H109" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I109" t="n">
         <v>6</v>
       </c>
       <c r="J109" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K109" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L109" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M109" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N109" t="n">
         <v>6</v>
@@ -6260,43 +6260,43 @@
         <v>45688</v>
       </c>
       <c r="B110" t="n">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C110" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D110" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E110" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F110" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G110" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H110" t="n">
         <v>1</v>
       </c>
       <c r="I110" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J110" t="n">
         <v>23</v>
       </c>
       <c r="K110" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L110" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M110" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N110" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O110" t="n">
         <v>0</v>
@@ -6313,40 +6313,40 @@
         <v>45716</v>
       </c>
       <c r="B111" t="n">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C111" t="n">
+        <v>26</v>
+      </c>
+      <c r="D111" t="n">
+        <v>8</v>
+      </c>
+      <c r="E111" t="n">
+        <v>11</v>
+      </c>
+      <c r="F111" t="n">
         <v>28</v>
-      </c>
-      <c r="D111" t="n">
-        <v>9</v>
-      </c>
-      <c r="E111" t="n">
-        <v>12</v>
-      </c>
-      <c r="F111" t="n">
-        <v>30</v>
       </c>
       <c r="G111" t="n">
         <v>8</v>
       </c>
       <c r="H111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I111" t="n">
         <v>6</v>
       </c>
       <c r="J111" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K111" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L111" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M111" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N111" t="n">
         <v>7</v>
@@ -6355,7 +6355,7 @@
         <v>0</v>
       </c>
       <c r="P111" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q111" t="n">
         <v>1</v>
@@ -6366,22 +6366,22 @@
         <v>45747</v>
       </c>
       <c r="B112" t="n">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C112" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D112" t="n">
+        <v>7</v>
+      </c>
+      <c r="E112" t="n">
+        <v>9</v>
+      </c>
+      <c r="F112" t="n">
+        <v>26</v>
+      </c>
+      <c r="G112" t="n">
         <v>8</v>
-      </c>
-      <c r="E112" t="n">
-        <v>10</v>
-      </c>
-      <c r="F112" t="n">
-        <v>28</v>
-      </c>
-      <c r="G112" t="n">
-        <v>9</v>
       </c>
       <c r="H112" t="n">
         <v>1</v>
@@ -6390,16 +6390,16 @@
         <v>5</v>
       </c>
       <c r="J112" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K112" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L112" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M112" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N112" t="n">
         <v>4</v>
@@ -6408,7 +6408,7 @@
         <v>0</v>
       </c>
       <c r="P112" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q112" t="n">
         <v>1</v>
@@ -6419,40 +6419,40 @@
         <v>45777</v>
       </c>
       <c r="B113" t="n">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C113" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D113" t="n">
         <v>7</v>
       </c>
       <c r="E113" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F113" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G113" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I113" t="n">
         <v>5</v>
       </c>
       <c r="J113" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K113" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L113" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M113" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N113" t="n">
         <v>4</v>
@@ -6472,19 +6472,19 @@
         <v>45808</v>
       </c>
       <c r="B114" t="n">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C114" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D114" t="n">
         <v>6</v>
       </c>
       <c r="E114" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F114" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G114" t="n">
         <v>8</v>
@@ -6496,16 +6496,16 @@
         <v>4</v>
       </c>
       <c r="J114" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K114" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L114" t="n">
         <v>11</v>
       </c>
       <c r="M114" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N114" t="n">
         <v>5</v>
@@ -6514,7 +6514,7 @@
         <v>0</v>
       </c>
       <c r="P114" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q114" t="n">
         <v>2</v>
@@ -6525,10 +6525,10 @@
         <v>45838</v>
       </c>
       <c r="B115" t="n">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C115" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D115" t="n">
         <v>8</v>
@@ -6537,7 +6537,7 @@
         <v>11</v>
       </c>
       <c r="F115" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G115" t="n">
         <v>8</v>
@@ -6549,28 +6549,28 @@
         <v>5</v>
       </c>
       <c r="J115" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K115" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L115" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M115" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N115" t="n">
+        <v>4</v>
+      </c>
+      <c r="O115" t="n">
+        <v>0</v>
+      </c>
+      <c r="P115" t="n">
         <v>5</v>
       </c>
-      <c r="O115" t="n">
-        <v>0</v>
-      </c>
-      <c r="P115" t="n">
-        <v>6</v>
-      </c>
       <c r="Q115" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116">
@@ -6578,52 +6578,52 @@
         <v>45869</v>
       </c>
       <c r="B116" t="n">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C116" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D116" t="n">
+        <v>7</v>
+      </c>
+      <c r="E116" t="n">
+        <v>10</v>
+      </c>
+      <c r="F116" t="n">
+        <v>33</v>
+      </c>
+      <c r="G116" t="n">
         <v>8</v>
       </c>
-      <c r="E116" t="n">
-        <v>11</v>
-      </c>
-      <c r="F116" t="n">
-        <v>35</v>
-      </c>
-      <c r="G116" t="n">
-        <v>9</v>
-      </c>
       <c r="H116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I116" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J116" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K116" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L116" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M116" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N116" t="n">
         <v>4</v>
       </c>
       <c r="O116" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P116" t="n">
         <v>6</v>
       </c>
       <c r="Q116" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117">
@@ -6631,52 +6631,52 @@
         <v>45900</v>
       </c>
       <c r="B117" t="n">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C117" t="n">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D117" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E117" t="n">
+        <v>16</v>
+      </c>
+      <c r="F117" t="n">
+        <v>59</v>
+      </c>
+      <c r="G117" t="n">
+        <v>11</v>
+      </c>
+      <c r="H117" t="n">
+        <v>1</v>
+      </c>
+      <c r="I117" t="n">
+        <v>7</v>
+      </c>
+      <c r="J117" t="n">
+        <v>28</v>
+      </c>
+      <c r="K117" t="n">
+        <v>42</v>
+      </c>
+      <c r="L117" t="n">
         <v>17</v>
       </c>
-      <c r="F117" t="n">
-        <v>63</v>
-      </c>
-      <c r="G117" t="n">
-        <v>12</v>
-      </c>
-      <c r="H117" t="n">
-        <v>2</v>
-      </c>
-      <c r="I117" t="n">
-        <v>8</v>
-      </c>
-      <c r="J117" t="n">
-        <v>30</v>
-      </c>
-      <c r="K117" t="n">
-        <v>45</v>
-      </c>
-      <c r="L117" t="n">
-        <v>18</v>
-      </c>
       <c r="M117" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N117" t="n">
         <v>5</v>
       </c>
       <c r="O117" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P117" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q117" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="118">
@@ -6684,19 +6684,19 @@
         <v>45930</v>
       </c>
       <c r="B118" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C118" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D118" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E118" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F118" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G118" t="n">
         <v>11</v>
@@ -6711,25 +6711,25 @@
         <v>25</v>
       </c>
       <c r="K118" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L118" t="n">
         <v>14</v>
       </c>
       <c r="M118" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N118" t="n">
         <v>6</v>
       </c>
       <c r="O118" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P118" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q118" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119">
@@ -6737,22 +6737,22 @@
         <v>45961</v>
       </c>
       <c r="B119" t="n">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C119" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D119" t="n">
+        <v>8</v>
+      </c>
+      <c r="E119" t="n">
+        <v>12</v>
+      </c>
+      <c r="F119" t="n">
+        <v>34</v>
+      </c>
+      <c r="G119" t="n">
         <v>7</v>
-      </c>
-      <c r="E119" t="n">
-        <v>10</v>
-      </c>
-      <c r="F119" t="n">
-        <v>27</v>
-      </c>
-      <c r="G119" t="n">
-        <v>5</v>
       </c>
       <c r="H119" t="n">
         <v>1</v>
@@ -6761,16 +6761,16 @@
         <v>4</v>
       </c>
       <c r="J119" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K119" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="L119" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M119" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N119" t="n">
         <v>5</v>
@@ -6779,10 +6779,10 @@
         <v>4</v>
       </c>
       <c r="P119" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q119" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>